<commit_message>
US14: Multiple Births Less Than 5
</commit_message>
<xml_diff>
--- a/Project-Sprint-Report.xlsx
+++ b/Project-Sprint-Report.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="190">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -934,11 +934,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="35055488"/>
-        <c:axId val="35057024"/>
+        <c:axId val="154682112"/>
+        <c:axId val="154683648"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="35055488"/>
+        <c:axId val="154682112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,14 +948,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35057024"/>
+        <c:crossAx val="154683648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="35057024"/>
+        <c:axId val="154683648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -966,7 +966,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35055488"/>
+        <c:crossAx val="154682112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2472,7 +2472,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
         <v>86</v>
@@ -2616,11 +2616,23 @@
       <c r="C7" t="s">
         <v>168</v>
       </c>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
       <c r="E7">
         <v>15</v>
       </c>
       <c r="F7">
         <v>20</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2688,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
us39: list upcoming anniversaries
</commit_message>
<xml_diff>
--- a/Project-Sprint-Report.xlsx
+++ b/Project-Sprint-Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="9510" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="9510" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="190">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -636,7 +636,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -676,6 +676,11 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -753,7 +758,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -780,6 +785,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="55"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -893,6 +900,9 @@
                 <c:pt idx="3">
                   <c:v>41197</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>41211</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -914,6 +924,9 @@
                 <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -934,11 +947,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="154682112"/>
-        <c:axId val="154683648"/>
+        <c:axId val="181661696"/>
+        <c:axId val="181663232"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="154682112"/>
+        <c:axId val="181661696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,14 +961,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154683648"/>
+        <c:crossAx val="181663232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="154683648"/>
+        <c:axId val="181663232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -966,7 +979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154682112"/>
+        <c:crossAx val="181661696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -977,7 +990,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1458,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1722,7 +1735,10 @@
         <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="E15" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1738,8 +1754,11 @@
       <c r="D16" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1752,8 +1771,11 @@
       <c r="D17" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1766,8 +1788,11 @@
       <c r="D18" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1780,8 +1805,11 @@
       <c r="D19" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1792,6 +1820,93 @@
         <v>110</v>
       </c>
       <c r="D20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1809,10 +1924,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1918,6 +2033,27 @@
       <c r="F5" s="9">
         <f>(D5-D4)/E5*60</f>
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>41211</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>860</v>
+      </c>
+      <c r="E6">
+        <v>320</v>
+      </c>
+      <c r="F6" s="9">
+        <f>(D6-D5)/E6*60</f>
+        <v>49.6875</v>
       </c>
     </row>
   </sheetData>
@@ -2176,7 +2312,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2471,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2511,7 +2647,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
         <v>110</v>
@@ -2519,11 +2655,23 @@
       <c r="C2" t="s">
         <v>167</v>
       </c>
+      <c r="D2" t="s">
+        <v>180</v>
+      </c>
       <c r="E2">
         <v>15</v>
       </c>
       <c r="F2">
         <v>10</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2536,11 +2684,23 @@
       <c r="C3" t="s">
         <v>166</v>
       </c>
+      <c r="D3" t="s">
+        <v>180</v>
+      </c>
       <c r="E3">
         <v>15</v>
       </c>
       <c r="F3">
         <v>10</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2582,11 +2742,23 @@
       <c r="C5" t="s">
         <v>167</v>
       </c>
+      <c r="D5" t="s">
+        <v>180</v>
+      </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5">
         <v>5</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -2599,11 +2771,23 @@
       <c r="C6" t="s">
         <v>166</v>
       </c>
+      <c r="D6" t="s">
+        <v>180</v>
+      </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6">
         <v>10</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2648,15 +2832,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2683,11 +2870,126 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2700,8 +3002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2898,6 +3200,9 @@
       <c r="C15" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="D15" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -2992,6 +3297,9 @@
       <c r="C23" s="12" t="s">
         <v>95</v>
       </c>
+      <c r="D23" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -3100,6 +3408,9 @@
       <c r="C32" s="12" t="s">
         <v>59</v>
       </c>
+      <c r="D32" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -3144,6 +3455,9 @@
       <c r="C36" s="12" t="s">
         <v>63</v>
       </c>
+      <c r="D36" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -3155,6 +3469,9 @@
       <c r="C37" s="12" t="s">
         <v>64</v>
       </c>
+      <c r="D37" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -3177,6 +3494,9 @@
       <c r="C39" s="12" t="s">
         <v>66</v>
       </c>
+      <c r="D39" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -3187,6 +3507,9 @@
       </c>
       <c r="C40" s="12" t="s">
         <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
US32: List Multiple Births
</commit_message>
<xml_diff>
--- a/Project-Sprint-Report.xlsx
+++ b/Project-Sprint-Report.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="190">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -947,11 +947,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="181661696"/>
-        <c:axId val="181663232"/>
+        <c:axId val="172932480"/>
+        <c:axId val="190391424"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="181661696"/>
+        <c:axId val="172932480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -961,14 +961,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181663232"/>
+        <c:crossAx val="190391424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="181663232"/>
+        <c:axId val="190391424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181661696"/>
+        <c:crossAx val="172932480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1016,7 +1016,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2835,7 +2835,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2916,11 +2916,23 @@
       <c r="C4" t="s">
         <v>168</v>
       </c>
+      <c r="D4" t="s">
+        <v>180</v>
+      </c>
       <c r="E4">
         <v>15</v>
       </c>
       <c r="F4">
         <v>20</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3002,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3422,6 +3434,9 @@
       <c r="C33" s="12" t="s">
         <v>60</v>
       </c>
+      <c r="D33" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">

</xml_diff>

<commit_message>
added use cases, need to fix 37, 38, 42
</commit_message>
<xml_diff>
--- a/Project-Sprint-Report.xlsx
+++ b/Project-Sprint-Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="9510" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="9510" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="190">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -604,12 +604,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
     <t>Refactoring Code</t>
   </si>
   <si>
@@ -626,6 +620,12 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>Output File</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -947,11 +947,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="172932480"/>
-        <c:axId val="190391424"/>
+        <c:axId val="143207808"/>
+        <c:axId val="143230080"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="172932480"/>
+        <c:axId val="143207808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -961,14 +961,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190391424"/>
+        <c:crossAx val="143230080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="190391424"/>
+        <c:axId val="143230080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172932480"/>
+        <c:crossAx val="143207808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1016,7 +1016,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1486,7 +1486,7 @@
     <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -1502,16 +1502,19 @@
       <c r="E1" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="D2" t="s">
         <v>166</v>
@@ -1519,16 +1522,19 @@
       <c r="E2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
         <v>166</v>
@@ -1536,33 +1542,39 @@
       <c r="E3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
         <v>168</v>
@@ -1570,33 +1582,39 @@
       <c r="E5" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
         <v>167</v>
@@ -1604,8 +1622,11 @@
       <c r="E7" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1621,8 +1642,11 @@
       <c r="E8" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1638,101 +1662,116 @@
       <c r="E9" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2</v>
-      </c>
+      <c r="F9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
         <v>168</v>
       </c>
-      <c r="E10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" t="s">
         <v>167</v>
       </c>
-      <c r="E11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
         <v>166</v>
       </c>
-      <c r="E12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" t="s">
-        <v>168</v>
-      </c>
       <c r="E13" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
         <v>168</v>
@@ -1740,107 +1779,131 @@
       <c r="E15" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E16" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
         <v>168</v>
       </c>
-      <c r="E17" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" t="s">
         <v>167</v>
       </c>
-      <c r="E18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" t="s">
-        <v>166</v>
-      </c>
       <c r="E19" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
         <v>155</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>110</v>
-      </c>
-      <c r="D20" t="s">
-        <v>167</v>
-      </c>
-      <c r="E20" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" t="s">
-        <v>118</v>
       </c>
       <c r="D21" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>180</v>
+      </c>
+      <c r="F21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1853,64 +1916,68 @@
       <c r="D22" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>60</v>
+        <v>157</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
       </c>
       <c r="D23" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
-        <v>161</v>
+      <c r="B24" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="E24" t="s">
+        <v>180</v>
+      </c>
+      <c r="F24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="E25" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F27">
+    <sortCondition ref="B2:B27"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2074,7 +2141,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2309,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2467,42 +2534,42 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
         <v>180</v>
@@ -2514,81 +2581,52 @@
         <v>10</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="I7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E8">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
-      <c r="H8">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I8" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
-        <v>31</v>
+      <c r="B13" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>184</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
+      <c r="B16" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
-        <v>32</v>
+      <c r="B17" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2608,7 +2646,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2834,8 +2872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3014,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3035,7 +3073,7 @@
         <v>71</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3060,7 +3098,7 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3074,7 +3112,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3088,7 +3126,7 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3102,7 +3140,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3116,7 +3154,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
@@ -3130,7 +3168,7 @@
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3166,7 +3204,7 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3213,7 +3251,7 @@
         <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3238,7 +3276,7 @@
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3296,7 +3334,7 @@
         <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3310,7 +3348,7 @@
         <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3368,7 +3406,7 @@
         <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3393,7 +3431,7 @@
         <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3407,7 +3445,7 @@
         <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3421,7 +3459,7 @@
         <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3435,7 +3473,7 @@
         <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3471,7 +3509,7 @@
         <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3485,7 +3523,7 @@
         <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3510,7 +3548,7 @@
         <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3524,7 +3562,7 @@
         <v>67</v>
       </c>
       <c r="D40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
@@ -3538,7 +3576,7 @@
         <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">

</xml_diff>